<commit_message>
Updated ReviewReport and Requirements
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\IdeaProjects\03_PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D4E0C6-80FB-4C94-A5FD-2D9840C6F147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB51A05-538C-4F13-8F0F-D377FB8EEF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="75">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -140,24 +140,6 @@
     <t>R01</t>
   </si>
   <si>
-    <t>R03</t>
-  </si>
-  <si>
-    <t>P01</t>
-  </si>
-  <si>
-    <t>P02</t>
-  </si>
-  <si>
-    <t>P05</t>
-  </si>
-  <si>
-    <t>O masa se poate elibera inainte de achitare</t>
-  </si>
-  <si>
-    <t>Cantitatea unei pizza este limitata la 5</t>
-  </si>
-  <si>
     <t>A02</t>
   </si>
   <si>
@@ -255,6 +237,30 @@
   </si>
   <si>
     <t>SonarQube</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>Se mentioneaza si folosirea butonului "ready" pentru notificare</t>
+  </si>
+  <si>
+    <t>F05</t>
+  </si>
+  <si>
+    <t>O masa ar trebui sa se poata elibera daca nu a fost facuta o comanda</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>F02 &amp; F03</t>
+  </si>
+  <si>
+    <t>Nu se specifica cum se initializeaza interfetele pentru bucataire si chelner</t>
   </si>
 </sst>
 </file>
@@ -484,6 +490,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -525,10 +535,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,8 +845,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -860,19 +866,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -885,8 +891,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>70</v>
+      <c r="I3" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="J3" s="17">
         <v>234</v>
@@ -896,15 +902,15 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>69</v>
+      <c r="I4" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
@@ -914,15 +920,15 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>71</v>
+      <c r="I5" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="J5" s="3">
         <v>234</v>
@@ -933,15 +939,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -965,50 +971,56 @@
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
@@ -1148,8 +1160,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,19 +1180,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1193,8 +1205,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>70</v>
+      <c r="I3" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="J3" s="17">
         <v>234</v>
@@ -1204,15 +1216,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>69</v>
+      <c r="I4" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
@@ -1222,15 +1234,15 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>71</v>
+      <c r="I5" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="J5" s="3">
         <v>234</v>
@@ -1241,15 +1253,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1270,13 +1282,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1285,13 +1297,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1300,13 +1312,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1465,7 +1477,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1486,19 +1498,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1511,8 +1523,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>70</v>
+      <c r="I3" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="J3" s="17">
         <v>234</v>
@@ -1522,15 +1534,15 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>69</v>
+      <c r="I4" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
@@ -1540,15 +1552,15 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>71</v>
+      <c r="I5" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="J5" s="3">
         <v>234</v>
@@ -1559,15 +1571,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1588,13 +1600,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1603,13 +1615,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1618,13 +1630,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1819,7 +1831,7 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
@@ -1841,19 +1853,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1866,8 +1878,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>70</v>
+      <c r="I3" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="J3" s="17">
         <v>234</v>
@@ -1877,15 +1889,15 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="31"/>
+      <c r="D4" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>69</v>
+      <c r="I4" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
@@ -1895,13 +1907,13 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>71</v>
+      <c r="I5" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="J5" s="3">
         <v>234</v>
@@ -1912,8 +1924,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1938,14 +1950,14 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1954,16 +1966,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1972,16 +1984,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1990,16 +2002,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2008,16 +2020,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2181,11 +2193,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="18">
         <v>0.3</v>
       </c>

</xml_diff>